<commit_message>
sua theo loi + quy dinh
</commit_message>
<xml_diff>
--- a/MauExcel.xlsx
+++ b/MauExcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Trang_Trai_Nuoi_Heo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D59FAD2-FCF0-4E48-AEB5-7DAE1FC48C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AB176D-535E-4637-A3B6-8D7E3822BFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="435" windowWidth="17940" windowHeight="11835" xr2:uid="{819DCD22-0DE8-4830-822C-F752579029D1}"/>
+    <workbookView xWindow="6315" yWindow="1260" windowWidth="17265" windowHeight="9960" xr2:uid="{819DCD22-0DE8-4830-822C-F752579029D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>GioiTinh</t>
   </si>
@@ -65,18 +65,9 @@
     <t>Cái</t>
   </si>
   <si>
-    <t>12/12/2022</t>
-  </si>
-  <si>
-    <t>Heo con</t>
-  </si>
-  <si>
     <t>NT001</t>
   </si>
   <si>
-    <t>Sức khỏe tốt</t>
-  </si>
-  <si>
     <t>Nhập ngoài</t>
   </si>
   <si>
@@ -87,6 +78,27 @@
   </si>
   <si>
     <t>Heo Ỉ Pha</t>
+  </si>
+  <si>
+    <t>Heo thịt</t>
+  </si>
+  <si>
+    <t>Heo Móng Cái</t>
+  </si>
+  <si>
+    <t>Heo Yorkshire</t>
+  </si>
+  <si>
+    <t>NT002</t>
+  </si>
+  <si>
+    <t>NT003</t>
+  </si>
+  <si>
+    <t>1/12/2022</t>
+  </si>
+  <si>
+    <t>Sức khoẻ tốt</t>
   </si>
 </sst>
 </file>
@@ -439,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBA0CB2-0357-4180-AEDB-3D5CA8E88EBF}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,10 +485,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -493,25 +505,77 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
-        <v>50</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>